<commit_message>
resultados finales entrega final para revison
</commit_message>
<xml_diff>
--- a/tarea 1/src/datos-estadistica/datos.xlsx
+++ b/tarea 1/src/datos-estadistica/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRISTIAN\Desktop\semestre_2024-2\estadistica lll\talleres\proyecto-PCA\tarea 1\src\datos-estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0D44BE-1238-4A6E-8888-238732BC67BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9257C6-918B-44C7-AE68-B3E8EBC0E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF297744-7B58-4192-83F8-D6F6694BA008}"/>
   </bookViews>
@@ -693,12 +693,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1BC459-F0D4-495A-A92B-FA8A630F195A}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="105" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
     <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
@@ -864,21 +865,21 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="D7" s="1">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
-        <v>7.3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9.1999999999999993</v>
-      </c>
       <c r="E7" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1">
         <v>52</v>
@@ -887,154 +888,154 @@
         <v>48</v>
       </c>
       <c r="H7" s="6">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>6.2</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="D8" s="1">
-        <v>12</v>
+        <v>11.6</v>
       </c>
       <c r="E8" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H8" s="6">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
-        <v>5.0999999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="C9" s="1">
-        <v>0.76</v>
+        <v>0.43</v>
       </c>
       <c r="D9" s="1">
-        <v>16.3</v>
+        <v>10.7</v>
       </c>
       <c r="E9" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H9" s="6">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>4.8</v>
+        <v>3.5</v>
       </c>
       <c r="C10" s="1">
-        <v>0.53</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="1">
-        <v>13.4</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" s="6">
-        <v>1.1000000000000001</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="C11" s="1">
-        <v>0.52</v>
+        <v>0.45</v>
       </c>
       <c r="D11" s="1">
-        <v>11.6</v>
+        <v>12.9</v>
       </c>
       <c r="E11" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G11" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" s="6">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>0.43</v>
+        <v>0.49</v>
       </c>
       <c r="D12" s="1">
-        <v>10.7</v>
+        <v>13.5</v>
       </c>
       <c r="E12" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F12" s="1">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H12" s="6">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="C13" s="1">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="D13" s="1">
-        <v>13</v>
+        <v>14.8</v>
       </c>
       <c r="E13" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F13" s="1">
         <v>51</v>
@@ -1043,24 +1044,24 @@
         <v>49</v>
       </c>
       <c r="H13" s="6">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C14" s="1">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="D14" s="1">
-        <v>12.9</v>
+        <v>14.1</v>
       </c>
       <c r="E14" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1">
         <v>52</v>
@@ -1069,99 +1070,99 @@
         <v>48</v>
       </c>
       <c r="H14" s="6">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C15" s="1">
-        <v>0.49</v>
+        <v>0.33</v>
       </c>
       <c r="D15" s="1">
-        <v>13.5</v>
+        <v>15.2</v>
       </c>
       <c r="E15" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F15" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G15" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" s="6">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
       <c r="C16" s="1">
-        <v>0.47</v>
+        <v>0.3</v>
       </c>
       <c r="D16" s="1">
-        <v>14.8</v>
+        <v>13.3</v>
       </c>
       <c r="E16" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F16" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G16" s="1">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H16" s="6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>0.35</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D17" s="1">
-        <v>14.1</v>
+        <v>16.5</v>
       </c>
       <c r="E17" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.8</v>
       </c>
       <c r="C18" s="1">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="D18" s="1">
-        <v>15.2</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1">
         <v>31</v>
@@ -1173,50 +1174,50 @@
         <v>48</v>
       </c>
       <c r="H18" s="6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1">
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
       <c r="C19" s="1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D19" s="1">
-        <v>13.3</v>
+        <v>17.5</v>
       </c>
       <c r="E19" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H19" s="6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C20" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.22</v>
       </c>
       <c r="D20" s="1">
-        <v>16.5</v>
+        <v>15.7</v>
       </c>
       <c r="E20" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F20" s="1">
         <v>51</v>
@@ -1225,24 +1226,24 @@
         <v>49</v>
       </c>
       <c r="H20" s="6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="D21" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="E21" s="1">
         <v>26</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="D21" s="1">
-        <v>10</v>
-      </c>
-      <c r="E21" s="1">
-        <v>31</v>
       </c>
       <c r="F21" s="1">
         <v>52</v>
@@ -1251,50 +1252,50 @@
         <v>48</v>
       </c>
       <c r="H21" s="6">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="D22" s="1">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1">
         <v>27</v>
       </c>
-      <c r="B22" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="F22" s="1">
+        <v>50</v>
+      </c>
+      <c r="G22" s="1">
+        <v>50</v>
+      </c>
+      <c r="H22" s="6">
         <v>0.2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>17.5</v>
-      </c>
-      <c r="E22" s="1">
-        <v>28</v>
-      </c>
-      <c r="F22" s="1">
-        <v>51</v>
-      </c>
-      <c r="G22" s="1">
-        <v>49</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C23" s="1">
-        <v>0.22</v>
+        <v>0.15</v>
       </c>
       <c r="D23" s="1">
-        <v>15.7</v>
+        <v>11.5</v>
       </c>
       <c r="E23" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F23" s="1">
         <v>51</v>
@@ -1303,128 +1304,128 @@
         <v>49</v>
       </c>
       <c r="H23" s="6">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1">
-        <v>0.13</v>
+        <v>0.05</v>
       </c>
       <c r="D24" s="1">
-        <v>18.2</v>
+        <v>13.6</v>
       </c>
       <c r="E24" s="1">
         <v>26</v>
       </c>
       <c r="F24" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G24" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H24" s="6">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="C25" s="1">
-        <v>0.08</v>
+        <v>0.01</v>
       </c>
       <c r="D25" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E25" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F25" s="1">
+        <v>51</v>
+      </c>
+      <c r="G25" s="1">
+        <v>49</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D26" s="8">
+        <v>22</v>
+      </c>
+      <c r="E26" s="8">
+        <v>28</v>
+      </c>
+      <c r="F26" s="8">
         <v>50</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G26" s="8">
         <v>50</v>
       </c>
-      <c r="H25" s="6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D26" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="E26" s="1">
-        <v>29</v>
-      </c>
-      <c r="F26" s="1">
-        <v>51</v>
-      </c>
-      <c r="G26" s="1">
-        <v>49</v>
-      </c>
-      <c r="H26" s="6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H26" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>7.3</v>
       </c>
       <c r="C27" s="1">
-        <v>0.05</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D27" s="1">
-        <v>13.6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E27" s="1">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F27" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G27" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H27" s="6">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B28" s="1">
-        <v>0.9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C28" s="1">
-        <v>0.08</v>
+        <v>0.76</v>
       </c>
       <c r="D28" s="1">
-        <v>12.2</v>
+        <v>16.3</v>
       </c>
       <c r="E28" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1">
         <v>51</v>
@@ -1433,24 +1434,24 @@
         <v>49</v>
       </c>
       <c r="H28" s="6">
-        <v>0.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B29" s="1">
-        <v>0.8</v>
+        <v>4.8</v>
       </c>
       <c r="C29" s="1">
-        <v>0.04</v>
+        <v>0.53</v>
       </c>
       <c r="D29" s="1">
-        <v>15</v>
+        <v>13.4</v>
       </c>
       <c r="E29" s="1">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F29" s="1">
         <v>52</v>
@@ -1459,59 +1460,59 @@
         <v>48</v>
       </c>
       <c r="H29" s="6">
-        <v>0.1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="C30" s="1">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D30" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1">
+        <v>26</v>
+      </c>
+      <c r="F30" s="1">
+        <v>52</v>
+      </c>
+      <c r="G30" s="1">
+        <v>48</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="D31" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="E31" s="1">
         <v>29</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F31" s="1">
         <v>51</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G31" s="1">
         <v>49</v>
       </c>
-      <c r="H30" s="6">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="C31" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="D31" s="8">
-        <v>22</v>
-      </c>
-      <c r="E31" s="8">
-        <v>28</v>
-      </c>
-      <c r="F31" s="8">
-        <v>50</v>
-      </c>
-      <c r="G31" s="8">
-        <v>50</v>
-      </c>
-      <c r="H31" s="9">
-        <v>0.05</v>
+      <c r="H31" s="6">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>